<commit_message>
atualização da sprint de python
</commit_message>
<xml_diff>
--- a/SPRINT_MATEMÁTICA/dados_user.xlsx
+++ b/SPRINT_MATEMÁTICA/dados_user.xlsx
@@ -477,19 +477,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>31.7</v>
+        <v>32.3</v>
       </c>
       <c r="F2" t="n">
-        <v>5.283333333333333</v>
+        <v>5.383333333333334</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -504,19 +504,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E3" t="n">
-        <v>18.5</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
-        <v>3.083333333333333</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -540,14 +540,14 @@
         <v>80</v>
       </c>
       <c r="E4" t="n">
-        <v>22.6</v>
+        <v>19.1</v>
       </c>
       <c r="F4" t="n">
-        <v>3.766666666666667</v>
+        <v>3.183333333333333</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>REPROVADO</t>
+          <t>APROVADO</t>
         </is>
       </c>
     </row>
@@ -558,19 +558,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E5" t="n">
-        <v>19.8</v>
+        <v>18</v>
       </c>
       <c r="F5" t="n">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>

</xml_diff>